<commit_message>
commit-0113 finalized data load
</commit_message>
<xml_diff>
--- a/assets/valuation_engine/Valuation_Engine_Mapping.xlsx
+++ b/assets/valuation_engine/Valuation_Engine_Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tao_project\dashboard_finance_metrics\assets\valuation_engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE762816-0BD1-4833-8DBA-7D14C8967F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12168D69-4848-4D77-9CA0-7347DD33329C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="722" firstSheet="1" activeTab="5" xr2:uid="{DB505F9D-00EE-40BB-9331-63CC137490AC}"/>
   </bookViews>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="507">
   <si>
     <t>is.net_revenue</t>
   </si>
@@ -898,12 +898,6 @@
     <t>(q_df.loc[index,'bs.total_assets']+q_df.loc[index-1,'bs.total_assets'])/(q_df.loc[index,'bs.total_shareholder_equity']+q_df.loc[index-1,'bs.total_shareholder_equity'])</t>
   </si>
   <si>
-    <t>q_df.loc[index,'is.operating_income']/q_df.loc[index,'is.interest_expense']</t>
-  </si>
-  <si>
-    <t>q_df.loc[index,'is.interest_expense']/q_df.loc[index,'is.operating_income']</t>
-  </si>
-  <si>
     <t>(q_df.loc[index,'is.net_revenue']-q_df.loc[index,'is.cost_of_sales'])/q_df.loc[index,'is.net_revenue']</t>
   </si>
   <si>
@@ -1604,6 +1598,15 @@
   </si>
   <si>
     <t>negative</t>
+  </si>
+  <si>
+    <t>q_df.loc[index,'is.operating_income']/abs(q_df.loc[index,'is.interest_expense'])</t>
+  </si>
+  <si>
+    <t>abs(q_df.loc[index,'is.interest_expense'])/q_df.loc[index,'is.operating_income']</t>
+  </si>
+  <si>
+    <t>multiple</t>
   </si>
 </sst>
 </file>
@@ -2147,7 +2150,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B11" t="s">
         <v>99</v>
@@ -2191,7 +2194,7 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
@@ -2611,10 +2614,10 @@
         <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H2" t="s">
         <v>44</v>
@@ -2623,19 +2626,19 @@
         <v>53</v>
       </c>
       <c r="J2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="K2" t="s">
         <v>47</v>
       </c>
       <c r="L2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="M2" t="s">
         <v>48</v>
       </c>
       <c r="N2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="O2" t="s">
         <v>51</v>
@@ -2644,7 +2647,7 @@
         <v>110</v>
       </c>
       <c r="Q2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -2652,31 +2655,31 @@
         <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="I3" t="s">
         <v>126</v>
       </c>
       <c r="J3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="L3" t="s">
         <v>46</v>
       </c>
       <c r="N3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="P3" t="s">
         <v>114</v>
@@ -2699,7 +2702,7 @@
         <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G4" t="s">
         <v>189</v>
@@ -2708,10 +2711,10 @@
         <v>153</v>
       </c>
       <c r="J4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="N4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="Q4" t="s">
         <v>52</v>
@@ -2719,7 +2722,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B5" t="s">
         <v>120</v>
@@ -2737,10 +2740,10 @@
         <v>43</v>
       </c>
       <c r="I5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="N5" t="s">
         <v>191</v>
@@ -2748,19 +2751,19 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F6" t="s">
         <v>76</v>
       </c>
       <c r="I6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="J6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="N6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -2768,10 +2771,10 @@
         <v>73</v>
       </c>
       <c r="J7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="N7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -2779,28 +2782,28 @@
         <v>190</v>
       </c>
       <c r="N8" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="N9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="N10" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="N11" t="s">
         <v>109</v>
@@ -2808,10 +2811,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="N12" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -2819,7 +2822,7 @@
         <v>131</v>
       </c>
       <c r="N13" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -2858,7 +2861,7 @@
     </row>
     <row r="19" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J19" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="20" spans="10:10" x14ac:dyDescent="0.25">
@@ -2873,7 +2876,7 @@
     </row>
     <row r="22" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J22" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" spans="10:10" x14ac:dyDescent="0.25">
@@ -2931,7 +2934,7 @@
         <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E2" t="s">
         <v>145</v>
@@ -2939,13 +2942,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C3" t="s">
         <v>132</v>
       </c>
       <c r="D3" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E3" t="s">
         <v>139</v>
@@ -2953,7 +2956,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C4" t="s">
         <v>64</v>
@@ -2962,18 +2965,18 @@
         <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D5" t="s">
         <v>155</v>
       </c>
       <c r="E5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2981,7 +2984,7 @@
         <v>112</v>
       </c>
       <c r="D6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
@@ -2997,15 +3000,15 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E8" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3015,12 +3018,12 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3101,10 +3104,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C2" t="s">
         <v>158</v>
@@ -3113,31 +3116,31 @@
         <v>159</v>
       </c>
       <c r="E2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I2" t="s">
         <v>135</v>
       </c>
       <c r="J2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="K2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="M2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3148,31 +3151,31 @@
         <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E3" t="s">
         <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G3" t="s">
         <v>151</v>
       </c>
       <c r="H3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I3" t="s">
         <v>118</v>
       </c>
       <c r="J3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="L3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="M3" t="s">
         <v>150</v>
@@ -3183,7 +3186,7 @@
         <v>199</v>
       </c>
       <c r="B4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C4" t="s">
         <v>56</v>
@@ -3192,28 +3195,28 @@
         <v>162</v>
       </c>
       <c r="F4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I4" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="J4" t="s">
         <v>128</v>
       </c>
       <c r="K4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L4" t="s">
+        <v>407</v>
+      </c>
+      <c r="M4" t="s">
         <v>409</v>
-      </c>
-      <c r="M4" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3233,24 +3236,24 @@
         <v>61</v>
       </c>
       <c r="I5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="J5" t="s">
         <v>62</v>
       </c>
       <c r="K5" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="L5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="M5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B6" t="s">
         <v>68</v>
@@ -3259,7 +3262,7 @@
         <v>142</v>
       </c>
       <c r="G6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I6" t="s">
         <v>127</v>
@@ -3268,13 +3271,13 @@
         <v>195</v>
       </c>
       <c r="K6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="M6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3294,10 +3297,10 @@
         <v>122</v>
       </c>
       <c r="K7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="L7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M7" t="s">
         <v>168</v>
@@ -3308,42 +3311,42 @@
         <v>143</v>
       </c>
       <c r="B8" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F8" t="s">
         <v>152</v>
       </c>
       <c r="G8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="I8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="K8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L8" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="M8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I9" t="s">
         <v>149</v>
       </c>
       <c r="K9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L9" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -3351,13 +3354,13 @@
         <v>146</v>
       </c>
       <c r="K10" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="L10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="M10" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -3365,46 +3368,46 @@
         <v>55</v>
       </c>
       <c r="K11" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L11" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="M11" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K12" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="L12" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="M12" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="L13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="M13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K14" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L14" t="s">
         <v>148</v>
       </c>
       <c r="M14" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -3412,21 +3415,21 @@
         <v>147</v>
       </c>
       <c r="L15" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="M15" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="L16" t="s">
         <v>130</v>
       </c>
       <c r="M16" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="11:13" x14ac:dyDescent="0.25">
@@ -3434,32 +3437,32 @@
         <v>129</v>
       </c>
       <c r="L17" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="M17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K18" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="L18" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="M18" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="19" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K19" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L19" t="s">
         <v>201</v>
       </c>
       <c r="M19" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="20" spans="11:13" x14ac:dyDescent="0.25">
@@ -3470,7 +3473,7 @@
         <v>134</v>
       </c>
       <c r="M20" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="11:13" x14ac:dyDescent="0.25">
@@ -3478,18 +3481,18 @@
         <v>134</v>
       </c>
       <c r="L21" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="M21" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="22" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K22" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="M22" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="23" spans="11:13" x14ac:dyDescent="0.25">
@@ -3504,17 +3507,17 @@
     </row>
     <row r="25" spans="11:13" x14ac:dyDescent="0.25">
       <c r="M25" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="26" spans="11:13" x14ac:dyDescent="0.25">
       <c r="M26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="11:13" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -3543,7 +3546,7 @@
         <v>188</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3581,7 +3584,7 @@
         <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3661,7 +3664,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G37" sqref="G37"/>
+      <selection pane="topRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3686,16 +3689,16 @@
         <v>222</v>
       </c>
       <c r="D1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="G1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3709,16 +3712,16 @@
         <v>223</v>
       </c>
       <c r="D2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F2" t="s">
+        <v>500</v>
+      </c>
+      <c r="G2" t="s">
         <v>502</v>
-      </c>
-      <c r="G2" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3732,16 +3735,16 @@
         <v>224</v>
       </c>
       <c r="D3" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F3" t="s">
+        <v>500</v>
+      </c>
+      <c r="G3" t="s">
         <v>502</v>
-      </c>
-      <c r="G3" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3749,22 +3752,22 @@
         <v>208</v>
       </c>
       <c r="B4" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C4" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D4" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E4" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F4" t="s">
+        <v>500</v>
+      </c>
+      <c r="G4" t="s">
         <v>502</v>
-      </c>
-      <c r="G4" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3778,16 +3781,16 @@
         <v>225</v>
       </c>
       <c r="D5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F5" t="s">
+        <v>500</v>
+      </c>
+      <c r="G5" t="s">
         <v>502</v>
-      </c>
-      <c r="G5" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3795,27 +3798,27 @@
         <v>210</v>
       </c>
       <c r="B6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C6" t="s">
         <v>227</v>
       </c>
       <c r="D6" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F6" t="s">
+        <v>500</v>
+      </c>
+      <c r="G6" t="s">
         <v>502</v>
-      </c>
-      <c r="G6" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B7" t="s">
         <v>229</v>
@@ -3824,21 +3827,21 @@
         <v>228</v>
       </c>
       <c r="D7" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E7" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F7" t="s">
+        <v>501</v>
+      </c>
+      <c r="G7" t="s">
         <v>503</v>
-      </c>
-      <c r="G7" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B8" t="s">
         <v>230</v>
@@ -3847,21 +3850,21 @@
         <v>231</v>
       </c>
       <c r="D8" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E8" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F8" t="s">
+        <v>501</v>
+      </c>
+      <c r="G8" t="s">
         <v>503</v>
-      </c>
-      <c r="G8" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B9" t="s">
         <v>233</v>
@@ -3870,21 +3873,21 @@
         <v>232</v>
       </c>
       <c r="D9" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E9" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F9" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="G9" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B10" t="s">
         <v>235</v>
@@ -3893,21 +3896,21 @@
         <v>234</v>
       </c>
       <c r="D10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E10" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F10" t="s">
+        <v>501</v>
+      </c>
+      <c r="G10" t="s">
         <v>503</v>
-      </c>
-      <c r="G10" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B11" t="s">
         <v>236</v>
@@ -3916,21 +3919,21 @@
         <v>237</v>
       </c>
       <c r="D11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E11" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F11" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="G11" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B12" t="s">
         <v>238</v>
@@ -3939,21 +3942,21 @@
         <v>239</v>
       </c>
       <c r="D12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F12" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="G12" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B13" t="s">
         <v>240</v>
@@ -3962,21 +3965,21 @@
         <v>242</v>
       </c>
       <c r="D13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E13" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="F13" t="s">
+        <v>500</v>
+      </c>
+      <c r="G13" t="s">
         <v>502</v>
-      </c>
-      <c r="G13" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B14" t="s">
         <v>241</v>
@@ -3985,21 +3988,21 @@
         <v>243</v>
       </c>
       <c r="D14" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E14" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="F14" t="s">
+        <v>500</v>
+      </c>
+      <c r="G14" t="s">
         <v>502</v>
-      </c>
-      <c r="G14" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B15" t="s">
         <v>266</v>
@@ -4008,21 +4011,21 @@
         <v>244</v>
       </c>
       <c r="D15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E15" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F15" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G15" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B16" t="s">
         <v>267</v>
@@ -4031,21 +4034,21 @@
         <v>246</v>
       </c>
       <c r="D16" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E16" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F16" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G16" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B17" t="s">
         <v>268</v>
@@ -4054,21 +4057,21 @@
         <v>245</v>
       </c>
       <c r="D17" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E17" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F17" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G17" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B18" t="s">
         <v>269</v>
@@ -4077,197 +4080,197 @@
         <v>247</v>
       </c>
       <c r="D18" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E18" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F18" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G18" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B19" t="s">
-        <v>270</v>
+        <v>504</v>
       </c>
       <c r="C19" t="s">
         <v>249</v>
       </c>
       <c r="D19" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E19" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F19" t="s">
+        <v>506</v>
+      </c>
+      <c r="G19" t="s">
         <v>502</v>
-      </c>
-      <c r="G19" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B20" t="s">
-        <v>271</v>
+        <v>505</v>
       </c>
       <c r="C20" t="s">
         <v>248</v>
       </c>
       <c r="D20" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E20" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F20" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G20" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B21" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C21" t="s">
         <v>250</v>
       </c>
       <c r="D21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E21" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F21" t="s">
+        <v>500</v>
+      </c>
+      <c r="G21" t="s">
         <v>502</v>
-      </c>
-      <c r="G21" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B22" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C22" t="s">
         <v>251</v>
       </c>
       <c r="D22" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E22" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F22" t="s">
+        <v>500</v>
+      </c>
+      <c r="G22" t="s">
         <v>502</v>
-      </c>
-      <c r="G22" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B23" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C23" t="s">
         <v>252</v>
       </c>
       <c r="D23" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E23" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F23" t="s">
+        <v>500</v>
+      </c>
+      <c r="G23" t="s">
         <v>502</v>
-      </c>
-      <c r="G23" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B24" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C24" t="s">
         <v>253</v>
       </c>
       <c r="D24" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E24" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F24" t="s">
+        <v>500</v>
+      </c>
+      <c r="G24" t="s">
         <v>502</v>
-      </c>
-      <c r="G24" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B25" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C25" t="s">
         <v>255</v>
       </c>
       <c r="D25" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E25" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F25" t="s">
+        <v>500</v>
+      </c>
+      <c r="G25" t="s">
         <v>502</v>
-      </c>
-      <c r="G25" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B26" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C26" t="s">
         <v>254</v>
       </c>
       <c r="D26" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E26" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F26" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G26" t="str">
         <f>$G$21</f>
@@ -4276,232 +4279,232 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B27" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C27" t="s">
         <v>256</v>
       </c>
       <c r="D27" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E27" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F27" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G27" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C28" t="s">
         <v>257</v>
       </c>
       <c r="D28" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E28" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F28" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G28" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B29" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C29" t="s">
         <v>258</v>
       </c>
       <c r="D29" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E29" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F29" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G29" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B30" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C30" t="s">
         <v>260</v>
       </c>
       <c r="D30" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E30" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F30" t="s">
+        <v>500</v>
+      </c>
+      <c r="G30" t="s">
         <v>502</v>
-      </c>
-      <c r="G30" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B31" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C31" t="s">
         <v>259</v>
       </c>
       <c r="D31" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E31" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F31" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G31" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B32" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C32" t="s">
         <v>261</v>
       </c>
       <c r="D32" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E32" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F32" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G32" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B33" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C33" t="s">
         <v>262</v>
       </c>
       <c r="D33" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E33" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F33" t="s">
+        <v>500</v>
+      </c>
+      <c r="G33" t="s">
         <v>502</v>
-      </c>
-      <c r="G33" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C34" t="s">
         <v>263</v>
       </c>
       <c r="D34" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E34" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F34" t="s">
+        <v>500</v>
+      </c>
+      <c r="G34" t="s">
         <v>502</v>
-      </c>
-      <c r="G34" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B35" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C35" t="s">
         <v>264</v>
       </c>
       <c r="D35" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E35" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F35" t="s">
+        <v>500</v>
+      </c>
+      <c r="G35" t="s">
         <v>502</v>
-      </c>
-      <c r="G35" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B36" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C36" t="s">
         <v>265</v>
       </c>
       <c r="D36" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E36" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F36" t="s">
+        <v>500</v>
+      </c>
+      <c r="G36" t="s">
         <v>502</v>
-      </c>
-      <c r="G36" t="s">
-        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -4524,7 +4527,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -4603,7 +4606,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B1">
         <v>1000000</v>
@@ -4611,7 +4614,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4619,7 +4622,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B3">
         <v>1000000</v>
@@ -4627,7 +4630,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B4">
         <v>1000</v>
@@ -4635,7 +4638,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -4643,7 +4646,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4651,7 +4654,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4659,7 +4662,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B8">
         <v>1000</v>
@@ -4686,7 +4689,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B1">
         <v>1000000</v>
@@ -4694,7 +4697,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B2">
         <v>1000000</v>
@@ -4702,7 +4705,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B3">
         <v>1000</v>
@@ -4710,7 +4713,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B4">
         <v>1000</v>
@@ -4718,7 +4721,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B5">
         <v>1000</v>
@@ -4726,7 +4729,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B6">
         <v>1000</v>
@@ -4734,7 +4737,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B7">
         <v>1000</v>

</xml_diff>